<commit_message>
Change class time to text
</commit_message>
<xml_diff>
--- a/data-transfer/data/cca/cca-class.xlsx
+++ b/data-transfer/data/cca/cca-class.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="104">
   <si>
     <t>Program</t>
   </si>
@@ -49,6 +49,9 @@
     <t>Wed</t>
   </si>
   <si>
+    <t>15:30</t>
+  </si>
+  <si>
     <t>1 hr</t>
   </si>
   <si>
@@ -61,12 +64,18 @@
     <t>Amanda</t>
   </si>
   <si>
+    <t>17:15</t>
+  </si>
+  <si>
     <t>B-Wed-01</t>
   </si>
   <si>
     <t>Tue</t>
   </si>
   <si>
+    <t>15:45</t>
+  </si>
+  <si>
     <t>B-Tue-01</t>
   </si>
   <si>
@@ -76,21 +85,39 @@
     <t>Sat</t>
   </si>
   <si>
+    <t>9:00</t>
+  </si>
+  <si>
     <t>B-Sat-01</t>
   </si>
   <si>
+    <t>10:15</t>
+  </si>
+  <si>
     <t>B-Sat-02</t>
   </si>
   <si>
+    <t>11:30</t>
+  </si>
+  <si>
     <t>B-Sat-03</t>
   </si>
   <si>
+    <t>13:30</t>
+  </si>
+  <si>
     <t>B-Sat-04</t>
   </si>
   <si>
+    <t>14:45</t>
+  </si>
+  <si>
     <t>B-Sat-05</t>
   </si>
   <si>
+    <t>16:00</t>
+  </si>
+  <si>
     <t>B-Sat-06</t>
   </si>
   <si>
@@ -106,6 +133,9 @@
     <t>Robbie</t>
   </si>
   <si>
+    <t>17:30</t>
+  </si>
+  <si>
     <t>B-Thu-01</t>
   </si>
   <si>
@@ -127,6 +157,9 @@
     <t>B-Sun-05</t>
   </si>
   <si>
+    <t>16:30</t>
+  </si>
+  <si>
     <t>B-Sun-06</t>
   </si>
   <si>
@@ -136,6 +169,9 @@
     <t>Kit</t>
   </si>
   <si>
+    <t>18:00</t>
+  </si>
+  <si>
     <t>2 hr</t>
   </si>
   <si>
@@ -148,6 +184,9 @@
     <t>Eli</t>
   </si>
   <si>
+    <t>15:00</t>
+  </si>
+  <si>
     <t>1.5 hr</t>
   </si>
   <si>
@@ -157,9 +196,15 @@
     <t>I-Wed-01</t>
   </si>
   <si>
+    <t>16:45</t>
+  </si>
+  <si>
     <t>I-Wed-03</t>
   </si>
   <si>
+    <t>17:00</t>
+  </si>
+  <si>
     <t>I-Tue-01</t>
   </si>
   <si>
@@ -190,6 +235,9 @@
     <t>I-Sat-04</t>
   </si>
   <si>
+    <t>15:15</t>
+  </si>
+  <si>
     <t>I-Sat-05</t>
   </si>
   <si>
@@ -202,12 +250,21 @@
     <t>I-Thu-01</t>
   </si>
   <si>
+    <t>8:45</t>
+  </si>
+  <si>
     <t>I-Sun-01</t>
   </si>
   <si>
+    <t>10:30</t>
+  </si>
+  <si>
     <t>I-Sun-02</t>
   </si>
   <si>
+    <t>13:00</t>
+  </si>
+  <si>
     <t>I-Sun-03</t>
   </si>
   <si>
@@ -229,6 +286,9 @@
     <t>A-Fri-02</t>
   </si>
   <si>
+    <t>10:45</t>
+  </si>
+  <si>
     <t>A-Sat-01</t>
   </si>
   <si>
@@ -245,6 +305,9 @@
   </si>
   <si>
     <t>Pre-AP/ AP</t>
+  </si>
+  <si>
+    <t>18:30</t>
   </si>
   <si>
     <t>AP-Wed-01</t>
@@ -349,7 +412,7 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -508,13 +571,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -613,10 +670,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -871,13 +928,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1190,10 +1241,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1503,17 +1554,17 @@
       <c r="D2" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E2" s="3">
-        <v>0.6458333333333333</v>
+      <c r="E2" t="s" s="3">
+        <v>12</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" ht="17" customHeight="1">
@@ -1524,22 +1575,22 @@
         <v>9</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E3" s="3">
-        <v>0.71875</v>
+      <c r="E3" t="s" s="3">
+        <v>17</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" ht="17" customHeight="1">
@@ -1553,19 +1604,19 @@
         <v>10</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.65625</v>
+        <v>19</v>
+      </c>
+      <c r="E4" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" ht="17" customHeight="1">
@@ -1576,22 +1627,22 @@
         <v>9</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.375</v>
+        <v>23</v>
+      </c>
+      <c r="E5" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" ht="17" customHeight="1">
@@ -1602,22 +1653,22 @@
         <v>9</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.4270833333333334</v>
+        <v>23</v>
+      </c>
+      <c r="E6" t="s" s="3">
+        <v>26</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" ht="17" customHeight="1">
@@ -1628,22 +1679,22 @@
         <v>9</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.4791666666666666</v>
+        <v>23</v>
+      </c>
+      <c r="E7" t="s" s="3">
+        <v>28</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" ht="17" customHeight="1">
@@ -1657,19 +1708,19 @@
         <v>10</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.5625</v>
+        <v>23</v>
+      </c>
+      <c r="E8" t="s" s="3">
+        <v>30</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" ht="17" customHeight="1">
@@ -1683,19 +1734,19 @@
         <v>10</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.6145833333333333</v>
+        <v>23</v>
+      </c>
+      <c r="E9" t="s" s="3">
+        <v>32</v>
       </c>
       <c r="F9" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H9" t="s" s="2">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" ht="17" customHeight="1">
@@ -1709,19 +1760,19 @@
         <v>10</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.6666666666666667</v>
+        <v>23</v>
+      </c>
+      <c r="E10" t="s" s="3">
+        <v>34</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" ht="17" customHeight="1">
@@ -1735,19 +1786,19 @@
         <v>10</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.71875</v>
+        <v>23</v>
+      </c>
+      <c r="E11" t="s" s="3">
+        <v>17</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" ht="17" customHeight="1">
@@ -1758,22 +1809,22 @@
         <v>9</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0.65625</v>
+        <v>37</v>
+      </c>
+      <c r="E12" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" ht="17" customHeight="1">
@@ -1784,22 +1835,22 @@
         <v>9</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.7291666666666667</v>
+        <v>37</v>
+      </c>
+      <c r="E13" t="s" s="3">
+        <v>40</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" ht="17" customHeight="1">
@@ -1810,22 +1861,22 @@
         <v>9</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.375</v>
+        <v>42</v>
+      </c>
+      <c r="E14" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" ht="17" customHeight="1">
@@ -1839,19 +1890,19 @@
         <v>10</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.4270833333333334</v>
+        <v>42</v>
+      </c>
+      <c r="E15" t="s" s="3">
+        <v>26</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" ht="17" customHeight="1">
@@ -1865,19 +1916,19 @@
         <v>10</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0.4791666666666666</v>
+        <v>42</v>
+      </c>
+      <c r="E16" t="s" s="3">
+        <v>28</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" ht="17" customHeight="1">
@@ -1891,19 +1942,19 @@
         <v>10</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0.5625</v>
+        <v>42</v>
+      </c>
+      <c r="E17" t="s" s="3">
+        <v>30</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H17" t="s" s="2">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" ht="17" customHeight="1">
@@ -1914,22 +1965,22 @@
         <v>9</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s" s="3">
         <v>32</v>
       </c>
-      <c r="E18" s="3">
-        <v>0.6145833333333333</v>
-      </c>
       <c r="F18" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H18" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" ht="17" customHeight="1">
@@ -1943,102 +1994,102 @@
         <v>10</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0.6875</v>
+        <v>42</v>
+      </c>
+      <c r="E19" t="s" s="3">
+        <v>48</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" ht="17" customHeight="1">
       <c r="A20" t="s" s="2">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0.75</v>
+        <v>23</v>
+      </c>
+      <c r="E20" t="s" s="3">
+        <v>52</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" ht="17" customHeight="1">
       <c r="A21" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E21" s="3">
-        <v>0.625</v>
+      <c r="E21" t="s" s="3">
+        <v>57</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" ht="17" customHeight="1">
       <c r="A22" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E22" s="3">
-        <v>0.6458333333333333</v>
+      <c r="E22" t="s" s="3">
+        <v>12</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H22" t="s" s="2">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" ht="17" customHeight="1">
       <c r="A23" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s" s="2">
         <v>9</v>
@@ -2049,22 +2100,22 @@
       <c r="D23" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E23" s="3">
-        <v>0.6979166666666667</v>
+      <c r="E23" t="s" s="3">
+        <v>61</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" ht="17" customHeight="1">
       <c r="A24" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s" s="2">
         <v>9</v>
@@ -2073,414 +2124,414 @@
         <v>10</v>
       </c>
       <c r="D24" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0.7083333333333333</v>
+        <v>19</v>
+      </c>
+      <c r="E24" t="s" s="3">
+        <v>63</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H24" t="s" s="2">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" ht="17" customHeight="1">
       <c r="A25" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="E25" s="3">
-        <v>0.65625</v>
+        <v>65</v>
+      </c>
+      <c r="E25" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" ht="17" customHeight="1">
       <c r="A26" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0.65625</v>
+        <v>65</v>
+      </c>
+      <c r="E26" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H26" t="s" s="2">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" ht="17" customHeight="1">
       <c r="A27" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="E27" s="3">
-        <v>0.7291666666666667</v>
+        <v>65</v>
+      </c>
+      <c r="E27" t="s" s="3">
+        <v>40</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H27" t="s" s="2">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" ht="17" customHeight="1">
       <c r="A28" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C28" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E28" s="3">
-        <v>0.375</v>
+        <v>23</v>
+      </c>
+      <c r="E28" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H28" t="s" s="2">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" ht="17" customHeight="1">
       <c r="A29" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E29" s="3">
-        <v>0.375</v>
+        <v>23</v>
+      </c>
+      <c r="E29" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" ht="17" customHeight="1">
       <c r="A30" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D30" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E30" s="3">
-        <v>0.5625</v>
+        <v>23</v>
+      </c>
+      <c r="E30" t="s" s="3">
+        <v>30</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>57</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" ht="17" customHeight="1">
       <c r="A31" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C31" t="s" s="2">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D31" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E31" s="3">
-        <v>0.5625</v>
+        <v>23</v>
+      </c>
+      <c r="E31" t="s" s="3">
+        <v>30</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" ht="17" customHeight="1">
       <c r="A32" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C32" t="s" s="2">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D32" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E32" s="3">
-        <v>0.6354166666666667</v>
+        <v>23</v>
+      </c>
+      <c r="E32" t="s" s="3">
+        <v>74</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" ht="17" customHeight="1">
       <c r="A33" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D33" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E33" s="3">
-        <v>0.7083333333333333</v>
+        <v>23</v>
+      </c>
+      <c r="E33" t="s" s="3">
+        <v>63</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" ht="17" customHeight="1">
       <c r="A34" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C34" t="s" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D34" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="E34" s="3">
-        <v>0.7083333333333333</v>
+        <v>37</v>
+      </c>
+      <c r="E34" t="s" s="3">
+        <v>63</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H34" t="s" s="2">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" ht="17" customHeight="1">
       <c r="A35" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C35" t="s" s="2">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D35" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="E35" s="3">
-        <v>0.65625</v>
+        <v>37</v>
+      </c>
+      <c r="E35" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H35" t="s" s="2">
-        <v>62</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" ht="17" customHeight="1">
       <c r="A36" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D36" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E36" s="3">
-        <v>0.3645833333333334</v>
+        <v>42</v>
+      </c>
+      <c r="E36" t="s" s="3">
+        <v>79</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H36" t="s" s="2">
-        <v>63</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" ht="17" customHeight="1">
       <c r="A37" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D37" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E37" s="3">
-        <v>0.4375</v>
+        <v>42</v>
+      </c>
+      <c r="E37" t="s" s="3">
+        <v>81</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H37" t="s" s="2">
-        <v>64</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" ht="17" customHeight="1">
       <c r="A38" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C38" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D38" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E38" s="3">
-        <v>0.5416666666666667</v>
+        <v>42</v>
+      </c>
+      <c r="E38" t="s" s="3">
+        <v>83</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H38" t="s" s="2">
-        <v>65</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" ht="17" customHeight="1">
       <c r="A39" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C39" t="s" s="2">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E39" s="3">
-        <v>0.5416666666666667</v>
+        <v>42</v>
+      </c>
+      <c r="E39" t="s" s="3">
+        <v>83</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H39" t="s" s="2">
-        <v>66</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" ht="17" customHeight="1">
       <c r="A40" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B40" t="s" s="2">
         <v>9</v>
@@ -2489,357 +2540,357 @@
         <v>10</v>
       </c>
       <c r="D40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="E40" t="s" s="3">
         <v>32</v>
       </c>
-      <c r="E40" s="3">
-        <v>0.6145833333333333</v>
-      </c>
       <c r="F40" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>67</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" ht="17" customHeight="1">
       <c r="A41" t="s" s="2">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D41" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E41" s="3">
-        <v>0.6979166666666667</v>
+      <c r="E41" t="s" s="3">
+        <v>61</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H41" t="s" s="2">
-        <v>69</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" ht="17" customHeight="1">
       <c r="A42" t="s" s="2">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B42" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D42" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="E42" s="3">
-        <v>0.65625</v>
+        <v>65</v>
+      </c>
+      <c r="E42" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H42" t="s" s="2">
-        <v>70</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" ht="17" customHeight="1">
       <c r="A43" t="s" s="2">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C43" t="s" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D43" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="E43" s="3">
-        <v>0.7291666666666667</v>
+        <v>65</v>
+      </c>
+      <c r="E43" t="s" s="3">
+        <v>40</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>71</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" ht="17" customHeight="1">
       <c r="A44" t="s" s="2">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B44" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C44" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D44" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E44" s="3">
-        <v>0.4479166666666666</v>
+        <v>23</v>
+      </c>
+      <c r="E44" t="s" s="3">
+        <v>91</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H44" t="s" s="2">
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" ht="17" customHeight="1">
       <c r="A45" t="s" s="2">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B45" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C45" t="s" s="2">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D45" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E45" s="3">
-        <v>0.4479166666666666</v>
+        <v>23</v>
+      </c>
+      <c r="E45" t="s" s="3">
+        <v>91</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H45" t="s" s="2">
-        <v>73</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" ht="17" customHeight="1">
       <c r="A46" t="s" s="2">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B46" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C46" t="s" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D46" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E46" s="3">
-        <v>0.6354166666666667</v>
+        <v>23</v>
+      </c>
+      <c r="E46" t="s" s="3">
+        <v>74</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H46" t="s" s="2">
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" ht="17" customHeight="1">
       <c r="A47" t="s" s="2">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C47" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D47" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E47" s="3">
-        <v>0.4375</v>
+        <v>42</v>
+      </c>
+      <c r="E47" t="s" s="3">
+        <v>81</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" ht="17" customHeight="1">
       <c r="A48" t="s" s="2">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D48" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="E48" t="s" s="3">
         <v>32</v>
       </c>
-      <c r="E48" s="3">
-        <v>0.6145833333333333</v>
-      </c>
       <c r="F48" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>76</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" ht="17" customHeight="1">
       <c r="A49" t="s" s="2">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="B49" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C49" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D49" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E49" s="3">
-        <v>0.7708333333333334</v>
+      <c r="E49" t="s" s="3">
+        <v>98</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>78</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" ht="17" customHeight="1">
       <c r="A50" t="s" s="2">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="B50" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C50" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D50" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E50" s="3">
-        <v>0.5625</v>
+        <v>23</v>
+      </c>
+      <c r="E50" t="s" s="3">
+        <v>30</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H50" t="s" s="2">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" ht="17" customHeight="1">
       <c r="A51" t="s" s="2">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="B51" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C51" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D51" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="E51" t="s" s="3">
         <v>20</v>
       </c>
-      <c r="E51" s="3">
-        <v>0.65625</v>
-      </c>
       <c r="F51" t="s" s="2">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H51" t="s" s="2">
-        <v>80</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" ht="17" customHeight="1">
       <c r="A52" t="s" s="2">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="B52" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C52" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D52" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E52" s="3">
-        <v>0.5416666666666667</v>
+        <v>42</v>
+      </c>
+      <c r="E52" t="s" s="3">
+        <v>83</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H52" t="s" s="2">
-        <v>81</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" ht="17" customHeight="1">
       <c r="A53" t="s" s="2">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="B53" t="s" s="2">
         <v>9</v>
       </c>
       <c r="C53" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D53" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E53" s="3">
-        <v>0.6354166666666667</v>
+        <v>42</v>
+      </c>
+      <c r="E53" t="s" s="3">
+        <v>74</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H53" t="s" s="2">
-        <v>82</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>